<commit_message>
add file reading practice
</commit_message>
<xml_diff>
--- a/apply/data/demo data/World_city.xlsx
+++ b/apply/data/demo data/World_city.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_home\python_tutorial\apply\data\demo data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC3DE0B3-9584-47F5-9ADB-DC5E2CF9347E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E219ADA-0398-40E2-841F-D0FA0BDEC986}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8F41A171-DC05-4ABE-BFA4-C95336118DA8}"/>
+    <workbookView xWindow="3660" yWindow="1605" windowWidth="15375" windowHeight="7875" xr2:uid="{3EE94FEB-C7DB-487A-A0DA-7B71D434EA1C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Asia" sheetId="1" r:id="rId1"/>
-    <sheet name="Europe" sheetId="3" r:id="rId2"/>
-    <sheet name="Africa" sheetId="2" r:id="rId3"/>
+    <sheet name="Asia" sheetId="2" r:id="rId1"/>
+    <sheet name="Europe" sheetId="1" r:id="rId2"/>
+    <sheet name="Africa" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,6 +50,63 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>London</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Britain</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Pairs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>France</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Berlin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Germany</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Moscow</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Russia</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Nigeria</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Abuja</t>
+  </si>
+  <si>
+    <t>Egypt</t>
+  </si>
+  <si>
+    <t>Cairo</t>
+  </si>
+  <si>
+    <t>Guinea</t>
+  </si>
+  <si>
+    <t>Conakry</t>
+  </si>
+  <si>
+    <t>Ethiopia</t>
+  </si>
+  <si>
+    <t>Addis Ababa</t>
+  </si>
+  <si>
     <t>China</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -58,92 +115,25 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>Japan</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>India</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Seoul</t>
+  </si>
+  <si>
+    <t>South Koera</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>New Delhi</t>
+  </si>
+  <si>
     <t>Tokyo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Japan</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Delhi</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>India</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>South Korea</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Seoul</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>London</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Britain</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>France</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pairs</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Germany</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Berlin</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Russia</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Moscow</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Egypt</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cairo</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>South Africa</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Pretoria</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Cameroon</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Yaoundé</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Uganda</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Kampala</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -506,11 +496,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35163778-F78F-4C66-A267-4AF354E6C297}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{01A45F4B-3CCC-4D49-85B1-236345FF3EAC}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -531,10 +521,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -542,10 +532,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -553,10 +543,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -564,10 +554,81 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DB8A83B-DB58-4135-AD0F-1A4A452306C2}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -577,12 +638,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7AFB21A-817C-40A3-BF4D-BEB827ED9EAE}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06789A1A-7C67-47D0-B6B2-289622A3099D}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -603,10 +664,10 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -640,77 +701,6 @@
       </c>
       <c r="C5" t="s">
         <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2066C57-26BE-4F0E-B0DC-57C322774CEC}">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>